<commit_message>
Add another author to the author .xlsx
</commit_message>
<xml_diff>
--- a/reports/masters_report/Chapter_4/author_moddelling_comparisson.xlsx
+++ b/reports/masters_report/Chapter_4/author_moddelling_comparisson.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balshaw\Desktop\Hybrid_Approach_To_Planetary_Gearbox_Prognostics\reports\masters_report\Chapter_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\douwm\repos\Hybrid_Approach_To_Planetary_Gearbox_Prognostics\reports\masters_report\Chapter_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6929804-CF19-400C-835F-E86F7EE6EBCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C3C205-249F-4B30-92D1-7ED5C564F84E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="-15750" windowWidth="26160" windowHeight="15225" xr2:uid="{C04A4BF8-D431-4013-836C-87B53AA7757D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C04A4BF8-D431-4013-836C-87B53AA7757D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
   <si>
     <t>Author</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Heath state</t>
   </si>
   <si>
-    <t>Heath state- Health indicator mapping</t>
-  </si>
-  <si>
     <t>Ellis 2019</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>Measured variable</t>
   </si>
   <si>
-    <t>Health indicator - Measured variable mapping</t>
-  </si>
-  <si>
     <t>Prognostics model implementation</t>
   </si>
   <si>
@@ -249,14 +243,47 @@
     <t>Health indicator, Condition indicator</t>
   </si>
   <si>
-    <t>Manipulation of measured variable</t>
+    <t>Processing of measured variable</t>
+  </si>
+  <si>
+    <t>Heath state- Health indicator mapping, fk</t>
+  </si>
+  <si>
+    <t>Health indicator - Measured variable mapping, hk</t>
+  </si>
+  <si>
+    <t>Spiral bevel gear degradation (pitting)</t>
+  </si>
+  <si>
+    <t>One dimensional transition function using whitening transform</t>
+  </si>
+  <si>
+    <t>Particle Filter with l-step ahead estimator</t>
+  </si>
+  <si>
+    <t>N/A This was buildt on data (ARIMA)</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>Oil debris</t>
+  </si>
+  <si>
+    <t>Oil debris, Acceleration</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Data driven Double exponential smoothing model</t>
+  </si>
+  <si>
+    <t>Check if this is summarized in lit review</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,8 +305,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +330,11 @@
         <fgColor theme="5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -306,13 +345,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -326,10 +366,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="1" builtinId="11"/>
   </cellStyles>
@@ -645,9 +687,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E0591CC-3AD8-4E33-8746-5A2B999F8F68}">
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C7" sqref="C7"/>
+      <selection pane="topRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,16 +707,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -683,25 +725,25 @@
         <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="O1" s="1"/>
       <c r="Q1" s="1"/>
@@ -714,119 +756,127 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="M3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="M5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -838,62 +888,66 @@
     </row>
     <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -905,77 +959,86 @@
     </row>
     <row r="10" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="M10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="F11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="M11" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E14" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inproved on He 2012 sections in chapter2 and .xlsx
</commit_message>
<xml_diff>
--- a/reports/masters_report/Chapter_4/author_moddelling_comparisson.xlsx
+++ b/reports/masters_report/Chapter_4/author_moddelling_comparisson.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balshaw\Desktop\Hybrid_Approach_To_Planetary_Gearbox_Prognostics\reports\masters_report\Chapter_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\douwm\repos\Hybrid_Approach_To_Planetary_Gearbox_Prognostics\reports\masters_report\Chapter_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128CA643-6241-4879-AA36-CB5588CC68DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C3C205-249F-4B30-92D1-7ED5C564F84E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="-15750" windowWidth="26160" windowHeight="15225" xr2:uid="{C04A4BF8-D431-4013-836C-87B53AA7757D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C04A4BF8-D431-4013-836C-87B53AA7757D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
   <si>
     <t>Author</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Heath state</t>
   </si>
   <si>
-    <t>Heath state- Health indicator mapping</t>
-  </si>
-  <si>
     <t>Ellis 2019</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>Measured variable</t>
   </si>
   <si>
-    <t>Health indicator - Measured variable mapping</t>
-  </si>
-  <si>
     <t>Prognostics model implementation</t>
   </si>
   <si>
@@ -249,14 +243,47 @@
     <t>Health indicator, Condition indicator</t>
   </si>
   <si>
-    <t>Manipulation of measured variable</t>
+    <t>Processing of measured variable</t>
+  </si>
+  <si>
+    <t>Heath state- Health indicator mapping, fk</t>
+  </si>
+  <si>
+    <t>Health indicator - Measured variable mapping, hk</t>
+  </si>
+  <si>
+    <t>Spiral bevel gear degradation (pitting)</t>
+  </si>
+  <si>
+    <t>One dimensional transition function using whitening transform</t>
+  </si>
+  <si>
+    <t>Particle Filter with l-step ahead estimator</t>
+  </si>
+  <si>
+    <t>N/A This was buildt on data (ARIMA)</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>Oil debris</t>
+  </si>
+  <si>
+    <t>Oil debris, Acceleration</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Data driven Double exponential smoothing model</t>
+  </si>
+  <si>
+    <t>Check if this is summarized in lit review</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,8 +305,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +330,11 @@
         <fgColor theme="5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -306,13 +345,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -326,10 +366,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="1" builtinId="11"/>
   </cellStyles>
@@ -645,9 +687,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E0591CC-3AD8-4E33-8746-5A2B999F8F68}">
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C7" sqref="C7"/>
+      <selection pane="topRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,16 +707,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -683,25 +725,25 @@
         <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="O1" s="1"/>
       <c r="Q1" s="1"/>
@@ -714,119 +756,127 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="M3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="M5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -838,62 +888,66 @@
     </row>
     <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -905,77 +959,86 @@
     </row>
     <row r="10" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="M10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="F11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="M11" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E14" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Order spectrum plotting and TSA oder spectrum plotting
</commit_message>
<xml_diff>
--- a/reports/masters_report/Chapter_4/author_moddelling_comparisson.xlsx
+++ b/reports/masters_report/Chapter_4/author_moddelling_comparisson.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balshaw\Desktop\Hybrid_Approach_To_Planetary_Gearbox_Prognostics\reports\masters_report\Chapter_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\douwm\repos\Hybrid_Approach_To_Planetary_Gearbox_Prognostics\reports\masters_report\Chapter_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6929804-CF19-400C-835F-E86F7EE6EBCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDA589B-53B0-4CAA-8920-8415886F8FDA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="-15750" windowWidth="26160" windowHeight="15225" xr2:uid="{C04A4BF8-D431-4013-836C-87B53AA7757D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C04A4BF8-D431-4013-836C-87B53AA7757D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
   <si>
     <t>Author</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Heath state</t>
   </si>
   <si>
-    <t>Heath state- Health indicator mapping</t>
-  </si>
-  <si>
     <t>Ellis 2019</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>Measured variable</t>
   </si>
   <si>
-    <t>Health indicator - Measured variable mapping</t>
-  </si>
-  <si>
     <t>Prognostics model implementation</t>
   </si>
   <si>
@@ -246,17 +240,50 @@
     <t>Saba et all 2009</t>
   </si>
   <si>
-    <t>Health indicator, Condition indicator</t>
-  </si>
-  <si>
-    <t>Manipulation of measured variable</t>
+    <t>Processing of measured variable</t>
+  </si>
+  <si>
+    <t>Heath state- Health indicator mapping, fk</t>
+  </si>
+  <si>
+    <t>Health indicator - Measured variable mapping, hk</t>
+  </si>
+  <si>
+    <t>Spiral bevel gear degradation (pitting)</t>
+  </si>
+  <si>
+    <t>Particle Filter with l-step ahead estimator</t>
+  </si>
+  <si>
+    <t>N/A This was buildt on data (ARIMA)</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Data driven Double exponential smoothing model</t>
+  </si>
+  <si>
+    <t>Check if this is summarized in lit review</t>
+  </si>
+  <si>
+    <t>One dimensional transition function using whitening transform, TSA many other CI's.</t>
+  </si>
+  <si>
+    <t>Oil debris mass</t>
+  </si>
+  <si>
+    <t>Health indicator, Condition indicator, Could be a difference between the two</t>
+  </si>
+  <si>
+    <t>Acceleration, Oli debris mass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,8 +305,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +330,11 @@
         <fgColor theme="5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -306,13 +345,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -326,10 +366,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="1" builtinId="11"/>
   </cellStyles>
@@ -645,9 +687,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E0591CC-3AD8-4E33-8746-5A2B999F8F68}">
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C7" sqref="C7"/>
+      <selection pane="topRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,16 +707,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -683,25 +725,25 @@
         <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="O1" s="1"/>
       <c r="Q1" s="1"/>
@@ -714,119 +756,127 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="M3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="M5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -838,62 +888,66 @@
     </row>
     <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -905,77 +959,86 @@
     </row>
     <row r="10" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="M10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="F11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="M11" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E14" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>